<commit_message>
Add Layout for Ambr parser, modify handling of NaN values in the parser, make necesssary changes in testing the parser, rename sheet names in the Ambr test file
</commit_message>
<xml_diff>
--- a/server/edd/load/tests/files/ambr_export_test_data.xlsx
+++ b/server/edd/load/tests/files/ambr_export_test_data.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/somtirtharoy/Downloads/ABPDU_EDD_import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/somtirtharoy/workspace/Projects/edd/server/edd/load/tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71777421-B5D6-EA46-83BE-04434ECC4D34}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42B8077-AE7B-5B4C-B488-6CE0842F35AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="920" windowWidth="26840" windowHeight="15540" xr2:uid="{BF9035A2-F3F4-9346-8C0D-CA9CB17C39E5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="HT1" sheetId="1" r:id="rId1"/>
+    <sheet name="HT2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>